<commit_message>
Testing commit to tracking-tables branch
</commit_message>
<xml_diff>
--- a/tracking_tables/confirmed_barriers_tracking_table_template.xlsx
+++ b/tracking_tables/confirmed_barriers_tracking_table_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cwffcf.sharepoint.com/sites/Conservation-General/Shared Documents/Freshwater/Fish Passage/General WCRP/Internal WCRP workshop (2023)/Table and list templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nWright\Documents\GitHub\wcrp-github-training\tracking_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{EE7B1C1A-57D3-4EDA-9629-CC1737274B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7162963-C1B6-4BC9-BAAA-80CE7CBADB7A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F003945-258B-4ADD-8C00-FF864D0CF1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13590" yWindow="0" windowWidth="13560" windowHeight="15615" activeTab="1" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed barriers" sheetId="1" r:id="rId1"/>
@@ -39,37 +39,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={92C847A6-92BE-4044-AC2C-B7E9CC68E97E}</author>
-    <author>tc={5D9EAF54-2CAE-4004-89C2-7FAA21041346}</author>
-    <author>tc={5BE5BED9-9B60-410F-BCE7-31A82DDCD128}</author>
     <author>tc={65A29B04-5B65-491E-80E8-7B589723DD09}</author>
   </authors>
   <commentList>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{92C847A6-92BE-4044-AC2C-B7E9CC68E97E}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    would need to be split up until the same number of columns as there are species/guilds</t>
-      </text>
-    </comment>
-    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{5D9EAF54-2CAE-4004-89C2-7FAA21041346}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    this would need to be avg gain for each species </t>
-      </text>
-    </comment>
-    <comment ref="R1" authorId="2" shapeId="0" xr:uid="{5BE5BED9-9B60-410F-BCE7-31A82DDCD128}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    this would need to be avg gain for each species </t>
-      </text>
-    </comment>
-    <comment ref="Y1" authorId="3" shapeId="0" xr:uid="{65A29B04-5B65-491E-80E8-7B589723DD09}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{65A29B04-5B65-491E-80E8-7B589723DD09}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -120,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Internal Name</t>
   </si>
@@ -128,12 +101,6 @@
     <t>Barrier ID (Crossing ID)</t>
   </si>
   <si>
-    <t>Watercourse Name</t>
-  </si>
-  <si>
-    <t>Road Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Easting </t>
   </si>
   <si>
@@ -143,39 +110,18 @@
     <t>Zone</t>
   </si>
   <si>
-    <t>Barrier Type</t>
-  </si>
-  <si>
     <t>Barrier Owner</t>
   </si>
   <si>
-    <t>Number of Downstream Barriers</t>
-  </si>
-  <si>
     <t>Assessment Type/Assessment Step Completed</t>
   </si>
   <si>
-    <t>Date of assesment</t>
-  </si>
-  <si>
-    <t>Passability status</t>
-  </si>
-  <si>
     <t>Partial passability notes</t>
   </si>
   <si>
     <t>Upstream habitat Quality</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Habitat Gain (km) </t>
-  </si>
-  <si>
-    <t>Habitat Gain (km) - spawning</t>
-  </si>
-  <si>
-    <t>Habitat Gain (km) - rearing</t>
-  </si>
-  <si>
     <t>Constructability</t>
   </si>
   <si>
@@ -206,9 +152,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>Column</t>
   </si>
   <si>
@@ -282,23 +225,31 @@
   </si>
   <si>
     <t>Engineering design</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Mine</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>CWF</t>
+  </si>
+  <si>
+    <t>LDN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -345,24 +296,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -691,16 +641,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="M1" dT="2024-01-25T16:17:13.21" personId="{99A25C25-CB7F-48CA-BD57-6FB272204657}" id="{92C847A6-92BE-4044-AC2C-B7E9CC68E97E}">
-    <text>would need to be split up until the same number of columns as there are species/guilds</text>
-  </threadedComment>
-  <threadedComment ref="Q1" dT="2024-01-25T16:15:44.96" personId="{99A25C25-CB7F-48CA-BD57-6FB272204657}" id="{5D9EAF54-2CAE-4004-89C2-7FAA21041346}">
-    <text xml:space="preserve">this would need to be avg gain for each species </text>
-  </threadedComment>
-  <threadedComment ref="R1" dT="2024-01-25T16:15:44.96" personId="{99A25C25-CB7F-48CA-BD57-6FB272204657}" id="{5BE5BED9-9B60-410F-BCE7-31A82DDCD128}">
-    <text xml:space="preserve">this would need to be avg gain for each species </text>
-  </threadedComment>
-  <threadedComment ref="Y1" dT="2024-02-15T14:52:52.95" personId="{99A25C25-CB7F-48CA-BD57-6FB272204657}" id="{65A29B04-5B65-491E-80E8-7B589723DD09}">
+  <threadedComment ref="P1" dT="2024-02-15T14:52:52.95" personId="{99A25C25-CB7F-48CA-BD57-6FB272204657}" id="{65A29B04-5B65-491E-80E8-7B589723DD09}">
     <text>Is there value in having a column for others involved that aren't leading?</text>
   </threadedComment>
 </ThreadedComments>
@@ -725,79 +666,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF604EB7-0D5F-45B2-A35A-2438164C3188}">
-  <dimension ref="A1:AB50"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1"/>
+      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="4" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="16" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" hidden="1" customWidth="1"/>
-    <col min="17" max="18" width="14.140625" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="14.140625" customWidth="1"/>
-    <col min="21" max="21" width="12.5703125" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" customWidth="1"/>
-    <col min="23" max="26" width="20.7109375" customWidth="1"/>
-    <col min="27" max="27" width="39.140625" customWidth="1"/>
-    <col min="28" max="28" width="51.5703125" customWidth="1"/>
+    <col min="1" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="26.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
+    <col min="10" max="11" width="14.1796875" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="14" max="17" width="20.7265625" customWidth="1"/>
+    <col min="18" max="18" width="39.1796875" customWidth="1"/>
+    <col min="19" max="19" width="51.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="44.25" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -815,83 +748,61 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L2" s="7">
+        <v>4.1673611111111111</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="O2" s="1">
+        <v>2025</v>
+      </c>
       <c r="P2" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28">
+        <v>44</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -911,17 +822,8 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28">
+    </row>
+    <row r="4" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -941,17 +843,8 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28">
+    </row>
+    <row r="5" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -971,17 +864,8 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:28">
+    </row>
+    <row r="6" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1001,17 +885,8 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="1:28">
+    </row>
+    <row r="7" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1031,17 +906,8 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28">
+    </row>
+    <row r="8" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1061,17 +927,8 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28">
+    </row>
+    <row r="9" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1091,17 +948,8 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28">
+    </row>
+    <row r="10" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1121,17 +969,8 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28">
+    </row>
+    <row r="11" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1151,17 +990,8 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28">
+    </row>
+    <row r="12" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1181,17 +1011,8 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="1:28">
+    </row>
+    <row r="13" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1211,17 +1032,8 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="1:28">
+    </row>
+    <row r="14" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1241,17 +1053,8 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-    </row>
-    <row r="15" spans="1:28">
+    </row>
+    <row r="15" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1271,17 +1074,8 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="1:28">
+    </row>
+    <row r="16" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1301,17 +1095,8 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-    </row>
-    <row r="17" spans="1:28">
+    </row>
+    <row r="17" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1331,180 +1116,171 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-    </row>
-    <row r="18" spans="1:28">
-      <c r="K18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="W18" s="1"/>
-    </row>
-    <row r="19" spans="1:28">
-      <c r="K19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="W19" s="1"/>
-    </row>
-    <row r="20" spans="1:28">
-      <c r="K20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="W20" s="1"/>
-    </row>
-    <row r="21" spans="1:28" ht="15" customHeight="1">
-      <c r="K21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="W21" s="1"/>
-    </row>
-    <row r="22" spans="1:28" ht="15" customHeight="1">
-      <c r="K22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="W22" s="1"/>
-    </row>
-    <row r="23" spans="1:28" ht="15" customHeight="1">
-      <c r="K23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="W23" s="1"/>
-    </row>
-    <row r="24" spans="1:28" ht="15" customHeight="1">
-      <c r="K24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="W24" s="1"/>
-    </row>
-    <row r="25" spans="1:28" ht="15" customHeight="1">
-      <c r="K25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="W25" s="1"/>
-    </row>
-    <row r="26" spans="1:28" ht="15" customHeight="1">
-      <c r="K26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="W26" s="1"/>
-    </row>
-    <row r="27" spans="1:28" ht="15" customHeight="1">
-      <c r="K27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="W27" s="1"/>
-    </row>
-    <row r="28" spans="1:28" ht="15" customHeight="1">
-      <c r="K28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="W28" s="1"/>
-    </row>
-    <row r="29" spans="1:28" ht="15" customHeight="1">
-      <c r="K29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="W29" s="1"/>
-    </row>
-    <row r="30" spans="1:28" ht="15" customHeight="1">
-      <c r="K30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="W30" s="1"/>
-    </row>
-    <row r="31" spans="1:28" ht="15" customHeight="1">
-      <c r="K31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="W31" s="1"/>
-    </row>
-    <row r="32" spans="1:28" ht="15" customHeight="1">
-      <c r="K32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="W32" s="1"/>
-    </row>
-    <row r="33" spans="11:23" ht="15" customHeight="1">
-      <c r="K33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="W33" s="1"/>
-    </row>
-    <row r="34" spans="11:23" ht="15" customHeight="1">
-      <c r="K34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="W34" s="1"/>
-    </row>
-    <row r="35" spans="11:23" ht="15" customHeight="1">
-      <c r="K35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="W35" s="1"/>
-    </row>
-    <row r="36" spans="11:23" ht="15" customHeight="1">
-      <c r="K36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="W36" s="1"/>
-    </row>
-    <row r="37" spans="11:23" ht="15" customHeight="1">
-      <c r="K37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="W37" s="1"/>
-    </row>
-    <row r="38" spans="11:23" ht="15" customHeight="1">
-      <c r="K38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="W38" s="1"/>
-    </row>
-    <row r="39" spans="11:23" ht="15" customHeight="1">
-      <c r="K39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="W39" s="1"/>
-    </row>
-    <row r="40" spans="11:23" ht="15" customHeight="1">
-      <c r="K40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="W40" s="1"/>
-    </row>
-    <row r="41" spans="11:23" ht="15" customHeight="1">
-      <c r="K41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="W41" s="1"/>
-    </row>
-    <row r="42" spans="11:23" ht="15" customHeight="1">
-      <c r="K42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="W42" s="1"/>
-    </row>
-    <row r="43" spans="11:23" ht="15" customHeight="1">
-      <c r="K43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="W43" s="1"/>
-    </row>
-    <row r="44" spans="11:23" ht="15" customHeight="1">
-      <c r="K44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="W44" s="1"/>
-    </row>
-    <row r="45" spans="11:23" ht="15" customHeight="1">
-      <c r="K45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="W45" s="1"/>
-    </row>
-    <row r="46" spans="11:23" ht="15" customHeight="1">
-      <c r="K46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="W46" s="1"/>
-    </row>
-    <row r="47" spans="11:23" ht="15" customHeight="1">
-      <c r="K47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="W47" s="1"/>
-    </row>
-    <row r="48" spans="11:23" ht="15" customHeight="1">
-      <c r="K48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="W48" s="1"/>
-    </row>
-    <row r="49" spans="11:23" ht="15" customHeight="1">
-      <c r="K49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="W49" s="1"/>
-    </row>
-    <row r="50" spans="11:23" ht="15" customHeight="1">
-      <c r="K50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="W50" s="1"/>
+    </row>
+    <row r="18" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="N38" s="1"/>
+    </row>
+    <row r="39" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="N42" s="1"/>
+    </row>
+    <row r="43" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="N44" s="1"/>
+    </row>
+    <row r="45" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="N46" s="1"/>
+    </row>
+    <row r="47" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="N47" s="1"/>
+    </row>
+    <row r="48" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="N48" s="1"/>
+    </row>
+    <row r="49" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="N49" s="1"/>
+    </row>
+    <row r="50" spans="7:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="N50" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1512,12 +1288,36 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{57410BA5-4960-471D-BD1B-0E835E03AF8A}">
           <x14:formula1>
-            <xm:f>Categories!#REF!</xm:f>
+            <xm:f>Categories!$B$3:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K50 W2:W50 V2 O2:O50</xm:sqref>
+          <xm:sqref>N2:N50</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{18DD9B67-20DA-44F5-9338-0786DEF02BF3}">
+          <x14:formula1>
+            <xm:f>Categories!$B$22:$B$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G50</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{90139091-22EA-4B04-A3C4-111390C800B8}">
+          <x14:formula1>
+            <xm:f>Categories!$B$17:$B$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I50</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B46066D4-D7A4-456B-9F27-11EEEC6A0E06}">
+          <x14:formula1>
+            <xm:f>Categories!$B$13:$B$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J50</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C59CE4C8-F1F5-4770-88F6-0EB58D002726}">
+          <x14:formula1>
+            <xm:f>Categories!$B$29:$B$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1527,175 +1327,190 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3499FD00-78FD-4500-A3A4-92452D91A23F}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A1:XFD17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="4" max="4" width="30.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
-      <c r="A2" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15">
-      <c r="A3" s="6"/>
-      <c r="B3" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="B5" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" ht="15">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15">
-      <c r="A16" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" ht="15">
-      <c r="A17" s="4"/>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15">
-      <c r="B20" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="B26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15"/>
-    <row r="28" spans="1:2" ht="15"/>
-    <row r="29" spans="1:2" ht="15"/>
-    <row r="30" spans="1:2" ht="15"/>
-    <row r="31" spans="1:2" ht="15"/>
-    <row r="32" spans="1:2" ht="15"/>
-    <row r="33" ht="15"/>
-    <row r="34" ht="15"/>
-    <row r="37" ht="15"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1703,6 +1518,37 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F2D6C6860AC114F8559403465E77CC4" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a456bade4bd732af03e24b44c1c2ca9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="411171ba-2276-4762-a69b-ae0a1d76a912" xmlns:ns3="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="630d1ab75a49860de5f9d74b152c7650" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1980,45 +1826,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B063947-0EE7-419B-A8E4-FA2F4F0C123E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
+    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B063947-0EE7-419B-A8E4-FA2F4F0C123E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
+    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Training update to confirmed barriers tracking table
</commit_message>
<xml_diff>
--- a/tracking_tables/confirmed_barriers_tracking_table_template.xlsx
+++ b/tracking_tables/confirmed_barriers_tracking_table_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cwffcf.sharepoint.com/sites/Conservation-General/Shared Documents/Freshwater/Fish Passage/General WCRP/Internal WCRP workshop (2023)/Table and list templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nWright\Documents\GitHub\wcrp-github-training\tracking_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="8_{EE7B1C1A-57D3-4EDA-9629-CC1737274B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4151F25-6D14-49DD-B361-E550853A39AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26621ABB-4B6E-4F8A-9762-01D9F5F60550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed barriers" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>Internal Name</t>
   </si>
@@ -193,6 +193,30 @@
   </si>
   <si>
     <t>Barrier type</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>Dam</t>
+  </si>
+  <si>
+    <t>Mine</t>
+  </si>
+  <si>
+    <t>CWF</t>
+  </si>
+  <si>
+    <t>LDN</t>
+  </si>
+  <si>
+    <t>Test.</t>
   </si>
 </sst>
 </file>
@@ -293,10 +317,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,9 +618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF604EB7-0D5F-45B2-A35A-2438164C3188}">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -688,28 +708,63 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+    <row r="2" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="1">
+        <v>5000</v>
+      </c>
       <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="1">
+        <v>2025</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
@@ -1451,6 +1506,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
@@ -1470,15 +1534,6 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1760,6 +1815,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1767,14 +1830,6 @@
     <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
     <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Changes for demo 2
Testing commit revert
</commit_message>
<xml_diff>
--- a/tracking_tables/confirmed_barriers_tracking_table_template.xlsx
+++ b/tracking_tables/confirmed_barriers_tracking_table_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\wcrp-github-training\tracking_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ACCE5F-4511-4F1F-B6BC-47EC318F599D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E20C06-677D-459D-997F-F7AC3650D1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31960" yWindow="-6280" windowWidth="26340" windowHeight="14150" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>Internal Name</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>for demo</t>
+  </si>
+  <si>
+    <t>Test 2</t>
   </si>
 </sst>
 </file>
@@ -623,7 +626,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -813,7 +816,9 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1529,6 +1534,37 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F2D6C6860AC114F8559403465E77CC4" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a456bade4bd732af03e24b44c1c2ca9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="411171ba-2276-4762-a69b-ae0a1d76a912" xmlns:ns3="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="630d1ab75a49860de5f9d74b152c7650" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1806,38 +1842,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
+    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B063947-0EE7-419B-A8E4-FA2F4F0C123E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1855,24 +1880,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA053DEA-D046-4166-9D26-72F5B44C5989}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
-    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Changes for demo 2"
This reverts commit 9060a88e38e0223d374214ee0308110b254fbebb.
</commit_message>
<xml_diff>
--- a/tracking_tables/confirmed_barriers_tracking_table_template.xlsx
+++ b/tracking_tables/confirmed_barriers_tracking_table_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\wcrp-github-training\tracking_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E20C06-677D-459D-997F-F7AC3650D1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ACCE5F-4511-4F1F-B6BC-47EC318F599D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31960" yWindow="-6280" windowWidth="26340" windowHeight="14150" xr2:uid="{BDE771D9-C9F3-45D6-96B6-E347CE1CFA3D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>Internal Name</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>for demo</t>
-  </si>
-  <si>
-    <t>Test 2</t>
   </si>
 </sst>
 </file>
@@ -626,7 +623,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -816,9 +813,7 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1534,37 +1529,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F2D6C6860AC114F8559403465E77CC4" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a456bade4bd732af03e24b44c1c2ca9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="411171ba-2276-4762-a69b-ae0a1d76a912" xmlns:ns3="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="630d1ab75a49860de5f9d74b152c7650" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1842,10 +1806,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="411171ba-2276-4762-a69b-ae0a1d76a912" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="411171ba-2276-4762-a69b-ae0a1d76a912">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B063947-0EE7-419B-A8E4-FA2F4F0C123E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
+    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1863,21 +1870,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B063947-0EE7-419B-A8E4-FA2F4F0C123E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A98FE5F-C603-4C27-8323-46B05BB00F7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
-    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>